<commit_message>
Fix for Report Filing
Fix for Report Filing
</commit_message>
<xml_diff>
--- a/Visulization Mappings/VisualizationMappings.xlsx
+++ b/Visulization Mappings/VisualizationMappings.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>CEO View</t>
   </si>
@@ -588,390 +588,6 @@
   </si>
   <si>
     <t>Filing Status on Finance Year</t>
-  </si>
-  <si>
-    <t>Balance Sheet Item</t>
-  </si>
-  <si>
-    <t>SEC XBRL Tag</t>
-  </si>
-  <si>
-    <t>Assets</t>
-  </si>
-  <si>
-    <t>Total Assets</t>
-  </si>
-  <si>
-    <t>Current Assets</t>
-  </si>
-  <si>
-    <t>AssetsCurrent</t>
-  </si>
-  <si>
-    <t>Cash &amp; Cash Equivalents</t>
-  </si>
-  <si>
-    <t>CashAndCashEquivalentsAtCarryingValue</t>
-  </si>
-  <si>
-    <t>Short-Term Investments</t>
-  </si>
-  <si>
-    <t>AvailableForSaleSecuritiesCurrent</t>
-  </si>
-  <si>
-    <t>Accounts Receivable</t>
-  </si>
-  <si>
-    <t>AccountsReceivableNetCurrent</t>
-  </si>
-  <si>
-    <t>Inventory</t>
-  </si>
-  <si>
-    <t>InventoryNet</t>
-  </si>
-  <si>
-    <t>Prepaid Expenses</t>
-  </si>
-  <si>
-    <t>PrepaidExpenseAndOtherAssetsCurrent</t>
-  </si>
-  <si>
-    <t>Non-Current Assets</t>
-  </si>
-  <si>
-    <t>AssetsNoncurrent</t>
-  </si>
-  <si>
-    <t>Property, Plant &amp; Equipment</t>
-  </si>
-  <si>
-    <t>PropertyPlantAndEquipmentNet</t>
-  </si>
-  <si>
-    <t>Intangible Assets (Goodwill, Patents, etc.)</t>
-  </si>
-  <si>
-    <t>Goodwill / IntangibleAssetsNetExcludingGoodwill</t>
-  </si>
-  <si>
-    <t>Long-Term Investments</t>
-  </si>
-  <si>
-    <t>AvailableForSaleSecuritiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Liabilities</t>
-  </si>
-  <si>
-    <t>Total Liabilities</t>
-  </si>
-  <si>
-    <t>Current Liabilities</t>
-  </si>
-  <si>
-    <t>LiabilitiesCurrent</t>
-  </si>
-  <si>
-    <t>Accounts Payable</t>
-  </si>
-  <si>
-    <t>AccountsPayableCurrent</t>
-  </si>
-  <si>
-    <t>Short-Term Debt</t>
-  </si>
-  <si>
-    <t>DebtCurrent</t>
-  </si>
-  <si>
-    <t>Accrued Liabilities</t>
-  </si>
-  <si>
-    <t>AccruedLiabilitiesCurrent</t>
-  </si>
-  <si>
-    <t>Deferred Revenue</t>
-  </si>
-  <si>
-    <t>DeferredRevenueCurrent</t>
-  </si>
-  <si>
-    <t>Long-Term Liabilities</t>
-  </si>
-  <si>
-    <t>LiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Long-Term Debt</t>
-  </si>
-  <si>
-    <t>LongTermDebtNoncurrent</t>
-  </si>
-  <si>
-    <t>Deferred Tax Liabilities</t>
-  </si>
-  <si>
-    <t>DeferredTaxLiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
-    <t>Total Shareholder Equity</t>
-  </si>
-  <si>
-    <t>StockholdersEquity / StockholdersEquityIncludingPortionAttributableToNoncontrollingInterest</t>
-  </si>
-  <si>
-    <t>Common Stock</t>
-  </si>
-  <si>
-    <t>CommonStockValue</t>
-  </si>
-  <si>
-    <t>Retained Earnings</t>
-  </si>
-  <si>
-    <t>RetainedEarningsAccumulatedDeficit</t>
-  </si>
-  <si>
-    <t>Additional Paid-in Capital</t>
-  </si>
-  <si>
-    <t>AdditionalPaidInCapital</t>
-  </si>
-  <si>
-    <t>Treasury Stock</t>
-  </si>
-  <si>
-    <t>TreasuryStockValue</t>
-  </si>
-  <si>
-    <t>Non-Controlling Interest</t>
-  </si>
-  <si>
-    <t>MinorityInter</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Assets ($M)</t>
-  </si>
-  <si>
-    <t>Liabilities + Equity ($M)</t>
-  </si>
-  <si>
-    <t>XBRL Tag</t>
-  </si>
-  <si>
-    <t>us-gaap:CashAndCashEquivalentsAtCarryingValue</t>
-  </si>
-  <si>
-    <t>us-gaap:MarketableSecuritiesCurrent</t>
-  </si>
-  <si>
-    <t>Accounts Receivable (Net)</t>
-  </si>
-  <si>
-    <t>us-gaap:AccountsReceivableNetCurrent</t>
-  </si>
-  <si>
-    <t>us-gaap:InventoryNet</t>
-  </si>
-  <si>
-    <t>Prepaid Expenses &amp; Other Current Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:PrepaidExpenseAndOtherAssetsCurrent</t>
-  </si>
-  <si>
-    <t>Deferred Tax Assets (Current)</t>
-  </si>
-  <si>
-    <t>us-gaap:DeferredTaxAssetsNetCurrent</t>
-  </si>
-  <si>
-    <t>Total Current Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:AssetsCurrent</t>
-  </si>
-  <si>
-    <t>Property, Plant &amp; Equipment (PPE, Net)</t>
-  </si>
-  <si>
-    <t>us-gaap:PropertyPlantAndEquipmentNet</t>
-  </si>
-  <si>
-    <t>us-gaap:MarketableSecuritiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Goodwill &amp; Intangible Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:Goodwill and us-gaap:IntangibleAssetsNetExcludingGoodwill</t>
-  </si>
-  <si>
-    <t>Operating Lease Right-of-Use Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:OperatingLeaseRightOfUseAsset</t>
-  </si>
-  <si>
-    <t>Deferred Tax Assets (Non-Current)</t>
-  </si>
-  <si>
-    <t>us-gaap:DeferredTaxAssetsNetNoncurrent</t>
-  </si>
-  <si>
-    <t>Other Non-Current Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:OtherAssetsNoncurrent</t>
-  </si>
-  <si>
-    <t>Total Non-Current Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:AssetsNoncurrent</t>
-  </si>
-  <si>
-    <t>TOTAL ASSETS</t>
-  </si>
-  <si>
-    <t>us-gaap:Assets</t>
-  </si>
-  <si>
-    <t>us-gaap:AccountsPayableCurrent</t>
-  </si>
-  <si>
-    <t>us-gaap:ShortTermBorrowings</t>
-  </si>
-  <si>
-    <t>Accrued Liabilities (Salaries, Taxes, etc.)</t>
-  </si>
-  <si>
-    <t>us-gaap:AccruedLiabilitiesCurrent</t>
-  </si>
-  <si>
-    <t>Lease Liabilities (Current)</t>
-  </si>
-  <si>
-    <t>us-gaap:OperatingLeaseLiabilityCurrent</t>
-  </si>
-  <si>
-    <t>Deferred Revenue (Short-Term)</t>
-  </si>
-  <si>
-    <t>us-gaap:DeferredRevenueCurrent</t>
-  </si>
-  <si>
-    <t>Income Taxes Payable</t>
-  </si>
-  <si>
-    <t>us-gaap:IncomeTaxesPayableCurrent</t>
-  </si>
-  <si>
-    <t>Total Current Liabilities</t>
-  </si>
-  <si>
-    <t>us-gaap:LiabilitiesCurrent</t>
-  </si>
-  <si>
-    <t>us-gaap:LongTermDebtNoncurrent</t>
-  </si>
-  <si>
-    <t>Lease Liabilities (Long-Term)</t>
-  </si>
-  <si>
-    <t>us-gaap:OperatingLeaseLiabilityNoncurrent</t>
-  </si>
-  <si>
-    <t>Deferred Revenue (Long-Term)</t>
-  </si>
-  <si>
-    <t>us-gaap:DeferredRevenueNoncurrent</t>
-  </si>
-  <si>
-    <t>Deferred Tax Liabilities (Non-Current)</t>
-  </si>
-  <si>
-    <t>us-gaap:DeferredTaxLiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Pension &amp; Other Employee Benefits</t>
-  </si>
-  <si>
-    <t>us-gaap:PensionAndOtherPostretirementBenefitsLiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Other Long-Term Liabilities</t>
-  </si>
-  <si>
-    <t>us-gaap:OtherLiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>Total Non-Current Liabilities</t>
-  </si>
-  <si>
-    <t>us-gaap:LiabilitiesNoncurrent</t>
-  </si>
-  <si>
-    <t>TOTAL LIABILITIES</t>
-  </si>
-  <si>
-    <t>us-gaap:Liabilities</t>
-  </si>
-  <si>
-    <t>us-gaap:CommonStockValue</t>
-  </si>
-  <si>
-    <t>Preferred Stock (if applicable)</t>
-  </si>
-  <si>
-    <t>us-gaap:PreferredStockValue</t>
-  </si>
-  <si>
-    <t>Additional Paid-In Capital (APIC)</t>
-  </si>
-  <si>
-    <t>us-gaap:AdditionalPaidInCapital</t>
-  </si>
-  <si>
-    <t>Treasury Stock (if applicable)</t>
-  </si>
-  <si>
-    <t>(-200)</t>
-  </si>
-  <si>
-    <t>us-gaap:TreasuryStockValue</t>
-  </si>
-  <si>
-    <t>us-gaap:RetainedEarningsAccumulatedDeficit</t>
-  </si>
-  <si>
-    <t>Accumulated Other Comprehensive Income (AOCI)</t>
-  </si>
-  <si>
-    <t>us-gaap:AccumulatedOtherComprehensiveIncomeLossNetOfTax</t>
-  </si>
-  <si>
-    <t>TOTAL STOCKHOLDERS' EQUITY</t>
-  </si>
-  <si>
-    <t>us-gaap:StockholdersEquityIncludingPortionAttributableToNoncontrollingInterest</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>us-gaap:LiabilitiesAndStockholdersEquity</t>
   </si>
 </sst>
 </file>
@@ -1648,24 +1264,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -2336,174 +1940,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="28.8" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" ht="43.2" spans="1:3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" ht="43.2" spans="1:3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" ht="43.2" spans="1:4">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" ht="86.4" spans="1:4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2519,7 +2123,7 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="B43" workbookViewId="0">
+    <sheetView topLeftCell="B14" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2532,174 +2136,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="28.8" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" ht="43.2" spans="1:3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" ht="43.2" spans="1:3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" ht="43.2" spans="1:4">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" ht="86.4" spans="1:4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2713,782 +2317,17 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="80.3333333333333" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="80.3333333333333" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.4444444444444" customWidth="1"/>
-    <col min="2" max="2" width="40.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="10.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="20.2222222222222" customWidth="1"/>
-    <col min="5" max="16384" width="80.3333333333333" customWidth="1"/>
+    <col min="1" max="16379" width="80.3333333333333" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" ht="43.2" spans="1:2">
-      <c r="A26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="3">
-        <v>500</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="3">
-        <v>200</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="3">
-        <v>600</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="3">
-        <v>450</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="3">
-        <v>150</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="3">
-        <v>50</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="4"/>
-      <c r="B41" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="5">
-        <v>1950</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="5">
-        <v>2500</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="3">
-        <v>800</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="5">
-        <v>1200</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="3">
-        <v>300</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="3">
-        <v>100</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="3">
-        <v>250</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="4"/>
-      <c r="B48" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="5">
-        <v>5150</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="4"/>
-      <c r="B49" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C49" s="5">
-        <v>7100</v>
-      </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="3">
-        <v>400</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="3">
-        <v>300</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="3">
-        <v>250</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="3">
-        <v>100</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="3">
-        <v>120</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="3">
-        <v>80</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="4"/>
-      <c r="B56" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5">
-        <v>1250</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5">
-        <v>1500</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="3">
-        <v>500</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="3">
-        <v>300</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="3">
-        <v>200</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="3">
-        <v>150</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="3">
-        <v>100</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="4"/>
-      <c r="B63" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="5">
-        <v>2750</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="4"/>
-      <c r="B64" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="5">
-        <v>4000</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="3">
-        <v>500</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="3">
-        <v>0</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="5">
-        <v>1500</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" ht="28.8" spans="1:5">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="3">
-        <v>300</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="4"/>
-      <c r="B71" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="5">
-        <v>3100</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="5">
-        <v>7100</v>
-      </c>
-      <c r="D72" s="5">
-        <v>7100</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>